<commit_message>
Se corregido errores al leer las notas en la pagina Estadisticas y se han añadido un txt de evaluacion y otro con atributos
</commit_message>
<xml_diff>
--- a/analisis-influencia-chatGPT/Ejemplos/Notas.xlsx
+++ b/analisis-influencia-chatGPT/Ejemplos/Notas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\Ejemplos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\Francis200202\analisis-influencia-chatGPT\analisis-influencia-chatGPT\Ejemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C2AF3C-8842-48D3-8D3C-7D709E650FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56C4E20-8C06-48AF-BD87-3304132F3FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{9C28DCF5-03D1-4A98-9276-A4EF562EFD29}"/>
   </bookViews>
@@ -93,19 +93,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Li"/>
     </font>
     <font>
       <sz val="11"/>
@@ -137,6 +131,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -164,24 +173,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,185 +529,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354B0112-8F46-4F85-B188-8E3F3674EDAB}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="8">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="8">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="15">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="8">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="15">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15">
-      <c r="A6" s="1" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="8">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15">
-      <c r="A7" s="1" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="15">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="8">
         <v>10</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15">
-      <c r="A8" s="1" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15">
-      <c r="A9" s="1" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="8">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15">
-      <c r="A10" s="1" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="8">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8">
         <v>7.15</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="15">
-      <c r="A11" s="1" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" ht="15">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="8">
+        <v>6</v>
+      </c>
+      <c r="C11" s="8">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15">
-      <c r="A12" s="1" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="8">
+        <v>6</v>
+      </c>
+      <c r="C12" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15">
-      <c r="A13" s="1" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="8">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="8">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15">
-      <c r="A14" s="1" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="8">
         <v>10</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="8">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15">
-      <c r="A15" s="1" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="8">
         <v>7</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -820,7 +861,8 @@
       <c r="C48" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se han modificado los ejemplos
</commit_message>
<xml_diff>
--- a/analisis-influencia-chatGPT/Ejemplos/Notas.xlsx
+++ b/analisis-influencia-chatGPT/Ejemplos/Notas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\source\repos\Francis200202\analisis-influencia-chatGPT\analisis-influencia-chatGPT\Ejemplos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franc\Desktop\analisis-influencia-ChatGPT\Ejemplos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56C4E20-8C06-48AF-BD87-3304132F3FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F674B7A1-CD69-47E4-850D-43DDBA19CD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{9C28DCF5-03D1-4A98-9276-A4EF562EFD29}"/>
+    <workbookView xWindow="-18300" yWindow="4020" windowWidth="17280" windowHeight="8880" xr2:uid="{9C28DCF5-03D1-4A98-9276-A4EF562EFD29}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
     <t>13 Nombre Apellido1 Apellido2</t>
   </si>
   <si>
-    <t>14 Nombre Apellido1 Apellido2</t>
+    <t>15 Nombre Apellido1 Apellido2</t>
   </si>
 </sst>
 </file>
@@ -531,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354B0112-8F46-4F85-B188-8E3F3674EDAB}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -727,10 +727,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C15" s="8">
-        <v>7</v>
+        <v>9.5</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>

</xml_diff>